<commit_message>
spanish and french language added
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_category.xlsx
+++ b/mosip_master/xlsx/doc_category.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21216" windowHeight="9084"/>
+    <workbookView windowWidth="18350" windowHeight="6920"/>
   </bookViews>
   <sheets>
-    <sheet name="data-1713953282198" sheetId="1" r:id="rId1"/>
+    <sheet name="doc_category" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
   <si>
     <t>code</t>
   </si>
@@ -71,85 +71,163 @@
     <t>Proof of Relationship</t>
   </si>
   <si>
+    <t>पते का प्रमाण</t>
+  </si>
+  <si>
+    <t>निवास प्रमाण पत्र</t>
+  </si>
+  <si>
+    <t>hin</t>
+  </si>
+  <si>
+    <t>सबूत की पहचान</t>
+  </si>
+  <si>
+    <t>पहचान प्रमाण</t>
+  </si>
+  <si>
+    <t>रिश्ते का सबूत</t>
+  </si>
+  <si>
+    <t>DocTestCode321</t>
+  </si>
+  <si>
+    <t>दॊच्चत्</t>
+  </si>
+  <si>
+    <t>दॊच्तॆस्त्चॊदॆ३२१ उप्दतॆद्</t>
+  </si>
+  <si>
+    <t>DocTestCode123</t>
+  </si>
+  <si>
+    <t>तॆस्तिन्ग् पॊसितिवॆ दॊच् उप्दतॆद्</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>Resident Photo</t>
+  </si>
+  <si>
+    <t>Proof of Resident Photo</t>
+  </si>
+  <si>
+    <t>POE</t>
+  </si>
+  <si>
+    <t>बायोमेट्रिक अपवाद का प्रमाण</t>
+  </si>
+  <si>
+    <t>Proof of Biometric Exception</t>
+  </si>
+  <si>
+    <t>POB</t>
+  </si>
+  <si>
+    <t>Proof of Birth</t>
+  </si>
+  <si>
+    <t>Proof date of birth of the person</t>
+  </si>
+  <si>
+    <t>जन्म का प्रमाण</t>
+  </si>
+  <si>
+    <t>व्यक्ति के जन्म की तारीख का प्रमाण</t>
+  </si>
+  <si>
+    <t>POF</t>
+  </si>
+  <si>
+    <t>Proof Of Foreigner</t>
+  </si>
+  <si>
+    <t>Proof of Foreigner Identity</t>
+  </si>
+  <si>
     <t>POC</t>
   </si>
   <si>
     <t>Proof of Consent</t>
   </si>
   <si>
-    <t>POE</t>
-  </si>
-  <si>
-    <t>Proof of Biometric Exception</t>
-  </si>
-  <si>
-    <t>पते का प्रमाण</t>
-  </si>
-  <si>
-    <t>निवास प्रमाण पत्र</t>
-  </si>
-  <si>
-    <t>hin</t>
-  </si>
-  <si>
-    <t>सबूत की पहचान</t>
-  </si>
-  <si>
-    <t>पहचान प्रमाण</t>
-  </si>
-  <si>
-    <t>रिश्ते का सबूत</t>
-  </si>
-  <si>
-    <t>बायोमेट्रिक अपवाद का प्रमाण</t>
-  </si>
-  <si>
-    <t>POB</t>
-  </si>
-  <si>
-    <t>Proof of Birth</t>
-  </si>
-  <si>
-    <t>Proof date of birth of the person</t>
-  </si>
-  <si>
-    <t>जन्म का प्रमाण</t>
-  </si>
-  <si>
-    <t>व्यक्ति के जन्म की तारीख का प्रमाण</t>
-  </si>
-  <si>
-    <t>DocTestCode321</t>
-  </si>
-  <si>
-    <t>दॊच्चत्</t>
-  </si>
-  <si>
-    <t>दॊच्तॆस्त्चॊदॆ३२१ उप्दतॆद्</t>
-  </si>
-  <si>
-    <t>DocTestCode123</t>
-  </si>
-  <si>
-    <t>तॆस्तिन्ग् पॊसितिवॆ दॊच् उप्दतॆद्</t>
-  </si>
-  <si>
-    <t>POP</t>
-  </si>
-  <si>
-    <t>Resident Photo</t>
-  </si>
-  <si>
-    <t>Proof of Resident Photo</t>
-  </si>
-  <si>
-    <t>POF</t>
-  </si>
-  <si>
-    <t>Proof Of Foreigner</t>
-  </si>
-  <si>
-    <t>Proof of Foreigner Identity</t>
+    <t>Comprobante de domicilio</t>
+  </si>
+  <si>
+    <t>Comprobante de dirección</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>Documentos de identidad</t>
+  </si>
+  <si>
+    <t>Prueba de identidad</t>
+  </si>
+  <si>
+    <t>Prueba de relación</t>
+  </si>
+  <si>
+    <t>Prueba de consentimiento</t>
+  </si>
+  <si>
+    <t>Prueba de excepción biométrica</t>
+  </si>
+  <si>
+    <t>Prueba de nacimiento</t>
+  </si>
+  <si>
+    <t>Prueba de fecha de nacimiento del persona</t>
+  </si>
+  <si>
+    <t>Foto residente</t>
+  </si>
+  <si>
+    <t>Foto de prueba de residente</t>
+  </si>
+  <si>
+    <t>Prueba de extranjero</t>
+  </si>
+  <si>
+    <t>Prueba de Identidad de Extranjero</t>
+  </si>
+  <si>
+    <t>Preuve d'adresse</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>Preuve d'identité</t>
+  </si>
+  <si>
+    <t>Preuve de relation</t>
+  </si>
+  <si>
+    <t>Preuve de consentement</t>
+  </si>
+  <si>
+    <t>Preuve d'exception biométrique</t>
+  </si>
+  <si>
+    <t>Preuve de naissance</t>
+  </si>
+  <si>
+    <t>Preuve de la date de naissance de la personne</t>
+  </si>
+  <si>
+    <t>Photo du résident</t>
+  </si>
+  <si>
+    <t>Preuve de photo de résidence</t>
+  </si>
+  <si>
+    <t>Preuve d'étranger</t>
+  </si>
+  <si>
+    <t>Preuve d'identité étrangère</t>
   </si>
 </sst>
 </file>
@@ -765,8 +843,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1302,13 +1386,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:F21"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.1818181818182" customWidth="1"/>
+    <col min="2" max="2" width="31.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="39.8181818181818" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -1327,7 +1416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1343,8 +1432,10 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1360,8 +1451,10 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1377,61 +1470,69 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -1440,123 +1541,147 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" s="1"/>
+      <c r="H10"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11"/>
+      <c r="G11" s="1"/>
+      <c r="H11"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12"/>
+      <c r="G12" s="1"/>
+      <c r="H12"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13"/>
+      <c r="G13" s="1"/>
+      <c r="H13"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14"/>
+      <c r="G14" s="1"/>
+      <c r="H14"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1564,13 +1689,17 @@
       <c r="E15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15"/>
+      <c r="G15" s="1"/>
+      <c r="H15"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -1579,6 +1708,282 @@
         <v>8</v>
       </c>
       <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16" s="1"/>
+      <c r="H16"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>